<commit_message>
Changing data in the Excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\misc\ng101\20221021\Api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\misc\ng101\20221021\API-Test-2023-01-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7358BA0C-4A9E-4972-AE7F-D9D1EC442517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9EDD3E-CD65-4A90-BA37-4D8B80B7006F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6BDB1C9C-F9F8-47F7-8823-8AFC58CFA2A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7875" xr2:uid="{6BDB1C9C-F9F8-47F7-8823-8AFC58CFA2A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
-    <t>title1</t>
-  </si>
-  <si>
     <t>title2</t>
   </si>
   <si>
@@ -86,18 +83,12 @@
     <t>icon</t>
   </si>
   <si>
-    <t>I have change this description right now</t>
-  </si>
-  <si>
     <t>This is the Second description</t>
   </si>
   <si>
     <t>bi bi-whatsapp</t>
   </si>
   <si>
-    <t>bi bi-tiktok</t>
-  </si>
-  <si>
     <t>Rabi3</t>
   </si>
   <si>
@@ -120,6 +111,15 @@
   </si>
   <si>
     <t>Rony-Rizk</t>
+  </si>
+  <si>
+    <t>Mohammad Ali Jarjoumah</t>
+  </si>
+  <si>
+    <t>Full Stack Web Developer</t>
+  </si>
+  <si>
+    <t>bi bi-linkedin</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,112 +492,112 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>